<commit_message>
prawie ostatnia wersja manuskryptu
</commit_message>
<xml_diff>
--- a/mlra-activity/data/final.xlsx
+++ b/mlra-activity/data/final.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_PROJECTS_\GIT\licencjat\mlra-activity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F54BC2-770F-49AD-81DB-C960725C31C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8158554F-B27B-4188-85CF-8135FD246968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="35216" windowHeight="19294" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="337" yWindow="3700" windowWidth="32801" windowHeight="14036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>sample</t>
   </si>
@@ -58,12 +58,6 @@
     <t>MlrA activity mU/mg protein</t>
   </si>
   <si>
-    <t>mean20</t>
-  </si>
-  <si>
-    <t>SEM20</t>
-  </si>
-  <si>
     <t>2022.04.07 - McC7 (ww2/3)</t>
   </si>
   <si>
@@ -164,6 +158,18 @@
   </si>
   <si>
     <t>K* 04.04</t>
+  </si>
+  <si>
+    <t>mean0</t>
+  </si>
+  <si>
+    <t>SEM0</t>
+  </si>
+  <si>
+    <t>mean1</t>
+  </si>
+  <si>
+    <t>SEM1</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC56"/>
+  <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -492,7 +498,7 @@
     <col min="1" max="1" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,65 +521,71 @@
         <v>6</v>
       </c>
       <c r="AB1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2">
         <v>2.6</v>
       </c>
       <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>16</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" t="s">
         <v>19</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
         <v>20</v>
       </c>
-      <c r="U2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" t="s">
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>21</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>23</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -624,24 +636,32 @@
         <v>2.4269688185291769</v>
       </c>
       <c r="W3">
-        <v>0.152412040346279</v>
+        <v>0.33214626770650979</v>
       </c>
       <c r="Y3">
-        <v>3.0482408069255802E-2</v>
+        <v>6.6429253541301955E-2</v>
       </c>
       <c r="AA3">
-        <v>79.618670972946816</v>
+        <v>36.534639321518569</v>
       </c>
       <c r="AB3">
-        <v>65.758306835352172</v>
+        <v>92.741776739239171</v>
       </c>
       <c r="AC3">
-        <v>10.340588597749555</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+        <v>56.207137417720595</v>
+      </c>
+      <c r="AD3">
+        <f>AVERAGE(Y3:Y5)</f>
+        <v>4.1361610695527663E-2</v>
+      </c>
+      <c r="AE3">
+        <f>_xlfn.STDEV.S(Y3:Y5)/SQRT(COUNT(Y3:Y5))</f>
+        <v>2.5067642845774295E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -688,19 +708,10 @@
       <c r="S4">
         <v>3.0649952077608278</v>
       </c>
-      <c r="W4">
-        <v>0.16825669128742701</v>
-      </c>
-      <c r="Y4">
-        <v>3.3651338257485404E-2</v>
-      </c>
-      <c r="AA4">
-        <v>72.121019376972981</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -748,18 +759,18 @@
         <v>2.4959446443920577</v>
       </c>
       <c r="W5">
-        <v>0.26649352712254798</v>
+        <v>8.1469839248766843E-2</v>
       </c>
       <c r="Y5">
-        <v>5.3298705424509596E-2</v>
+        <v>1.6293967849753368E-2</v>
       </c>
       <c r="AA5">
-        <v>45.535230156136713</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+        <v>148.94891415695977</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -810,10 +821,10 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>1.6863042874340213</v>
+        <v>0.21516393442623</v>
       </c>
       <c r="Y6">
-        <v>0.33726085748680423</v>
+        <v>4.3032786885245998E-2</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -824,10 +835,18 @@
       <c r="AC6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD6">
+        <f t="shared" ref="AD6" si="0">AVERAGE(Y6:Y8)</f>
+        <v>5.5288078943180052E-2</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6" si="1">_xlfn.STDEV.S(Y6:Y8)/SQRT(COUNT(Y6:Y8))</f>
+        <v>6.2031434887490234E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -875,18 +894,18 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>1.7835355125474577</v>
+        <v>0.29872274391214398</v>
       </c>
       <c r="Y7">
-        <v>0.35670710250949156</v>
+        <v>5.9744548782428797E-2</v>
       </c>
       <c r="AA7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -934,18 +953,18 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>1.6863042874340213</v>
+        <v>0.31543450580932686</v>
       </c>
       <c r="Y8">
-        <v>0.33726085748680423</v>
+        <v>6.3086901161865369E-2</v>
       </c>
       <c r="AA8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -996,24 +1015,32 @@
         <v>8.6994973342752502</v>
       </c>
       <c r="W9">
-        <v>3.3197888693397539</v>
+        <v>1.7631469115191989</v>
       </c>
       <c r="Y9">
-        <v>0.66395777386795074</v>
+        <v>0.35262938230383978</v>
       </c>
       <c r="AA9">
-        <v>13.102485845742088</v>
+        <v>24.670369999909454</v>
       </c>
       <c r="AB9">
-        <v>13.949232350431275</v>
+        <v>27.588529242041631</v>
       </c>
       <c r="AC9">
-        <v>0.46628741958416053</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+        <v>1.626397246442213</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" ref="AD9" si="2">AVERAGE(Y9:Y11)</f>
+        <v>0.31757095158597665</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" ref="AE9" si="3">_xlfn.STDEV.S(Y9:Y11)/SQRT(COUNT(Y9:Y11))</f>
+        <v>1.9035624276036587E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -1061,18 +1088,18 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>3.0993980924159641</v>
+        <v>1.5644824707846412</v>
       </c>
       <c r="Y10">
-        <v>0.61987961848319284</v>
+        <v>0.31289649415692822</v>
       </c>
       <c r="AA10">
-        <v>14.034172240672122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+        <v>27.803115396723356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1120,18 +1147,18 @@
         <v>17.705114247157354</v>
       </c>
       <c r="W11">
-        <v>2.956792295582924</v>
+        <v>1.4359348914858097</v>
       </c>
       <c r="Y11">
-        <v>0.5913584591165848</v>
+        <v>0.28718697829716194</v>
       </c>
       <c r="AA11">
-        <v>14.711038964879618</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+        <v>30.292102329492078</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1181,25 +1208,24 @@
       <c r="U12">
         <v>10.014309663446102</v>
       </c>
-      <c r="W12">
-        <v>5.2664250332245937</v>
-      </c>
-      <c r="Y12">
-        <v>1.0532850066449186</v>
-      </c>
-      <c r="AA12">
-        <v>9.5076922203090906</v>
-      </c>
       <c r="AB12">
-        <v>10.895986476218496</v>
+        <v>28.943811087016336</v>
       </c>
       <c r="AC12">
-        <v>0.99951352013708605</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+        <v>2.4746594558890731</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" ref="AD12" si="4">AVERAGE(Y12:Y14)</f>
+        <v>0.3485392320534223</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" ref="AE12" si="5">_xlfn.STDEV.S(Y12:Y14)/SQRT(COUNT(Y12:Y14))</f>
+        <v>2.9799666110183611E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -1247,18 +1273,18 @@
         <v>14.704665822122021</v>
       </c>
       <c r="W13">
-        <v>4.8403950706777774</v>
+        <v>1.8916944908180298</v>
       </c>
       <c r="Y13">
-        <v>0.96807901413555553</v>
+        <v>0.37833889816360594</v>
       </c>
       <c r="AA13">
-        <v>10.344516839246188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+        <v>26.469151631127264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -1306,18 +1332,18 @@
         <v>6.6344941961649262</v>
       </c>
       <c r="W14">
-        <v>3.9009443840360807</v>
+        <v>1.5936978297161937</v>
       </c>
       <c r="Y14">
-        <v>0.78018887680721616</v>
+        <v>0.31873956594323871</v>
       </c>
       <c r="AA14">
-        <v>12.835750369100209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+        <v>31.418470542905411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -1365,10 +1391,10 @@
         <v>0.12814913328336572</v>
       </c>
       <c r="W15">
-        <v>3.3197888693397539</v>
+        <v>1.7631469115191989</v>
       </c>
       <c r="Y15">
-        <v>0.66395777386795074</v>
+        <v>0.35262938230383978</v>
       </c>
       <c r="AA15">
         <v>0</v>
@@ -1379,10 +1405,18 @@
       <c r="AC15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD15">
+        <f t="shared" ref="AD15" si="6">AVERAGE(Y15:Y17)</f>
+        <v>0.31757095158597665</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" ref="AE15" si="7">_xlfn.STDEV.S(Y15:Y17)/SQRT(COUNT(Y15:Y17))</f>
+        <v>1.9035624276036587E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>100</v>
@@ -1430,18 +1464,18 @@
         <v>0.12814913328336572</v>
       </c>
       <c r="W16">
-        <v>3.0993980924159641</v>
+        <v>1.5644824707846412</v>
       </c>
       <c r="Y16">
-        <v>0.61987961848319284</v>
+        <v>0.31289649415692822</v>
       </c>
       <c r="AA16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>100</v>
@@ -1489,18 +1523,18 @@
         <v>0.12814913328336572</v>
       </c>
       <c r="W17">
-        <v>2.956792295582924</v>
+        <v>1.4359348914858097</v>
       </c>
       <c r="Y17">
-        <v>0.5913584591165848</v>
+        <v>0.28718697829716194</v>
       </c>
       <c r="AA17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>100</v>
@@ -1547,25 +1581,24 @@
       <c r="S18">
         <v>0.12814913328336572</v>
       </c>
-      <c r="W18">
-        <v>5.2664250332245937</v>
-      </c>
-      <c r="Y18">
-        <v>1.0532850066449186</v>
-      </c>
-      <c r="AA18">
-        <v>0</v>
-      </c>
       <c r="AB18">
         <v>0</v>
       </c>
       <c r="AC18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD18">
+        <f t="shared" ref="AD18" si="8">AVERAGE(Y18:Y20)</f>
+        <v>0.3485392320534223</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" ref="AE18" si="9">_xlfn.STDEV.S(Y18:Y20)/SQRT(COUNT(Y18:Y20))</f>
+        <v>2.9799666110183611E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <v>100</v>
@@ -1613,18 +1646,18 @@
         <v>0.12814913328336572</v>
       </c>
       <c r="W19">
-        <v>4.8403950706777774</v>
+        <v>1.8916944908180298</v>
       </c>
       <c r="Y19">
-        <v>0.96807901413555553</v>
+        <v>0.37833889816360594</v>
       </c>
       <c r="AA19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20">
         <v>100</v>
@@ -1672,18 +1705,18 @@
         <v>0.12814913328336572</v>
       </c>
       <c r="W20">
-        <v>3.9009443840360807</v>
+        <v>1.5936978297161937</v>
       </c>
       <c r="Y20">
-        <v>0.78018887680721616</v>
+        <v>0.31873956594323871</v>
       </c>
       <c r="AA20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -1734,24 +1767,32 @@
         <v>20.653830802795522</v>
       </c>
       <c r="W21">
-        <v>0.152412040346279</v>
+        <v>0.47416704187303016</v>
       </c>
       <c r="Y21">
-        <v>3.0482408069255802E-2</v>
+        <v>9.4833408374606035E-2</v>
       </c>
       <c r="AA21">
-        <v>79.618670972946816</v>
+        <v>25.591918081677399</v>
       </c>
       <c r="AB21">
-        <v>75.869845174959892</v>
+        <v>23.469815963518506</v>
       </c>
       <c r="AC21">
-        <v>3.7488257979869171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+        <v>2.1221021181588924</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" ref="AD21" si="10">AVERAGE(Y21:Y23)</f>
+        <v>0.10426046825754165</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" ref="AE21" si="11">_xlfn.STDEV.S(Y21:Y23)/SQRT(COUNT(Y21:Y23))</f>
+        <v>9.4270598829356081E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -1799,30 +1840,30 @@
         <v>20.653830802795522</v>
       </c>
       <c r="W22">
-        <v>0.16825669128742701</v>
+        <v>0.56843764070238623</v>
       </c>
       <c r="Y22">
-        <v>3.3651338257485404E-2</v>
+        <v>0.11368752814047725</v>
       </c>
       <c r="AA22">
-        <v>72.121019376972981</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+        <v>21.347713845359614</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
         <v>27</v>
-      </c>
-      <c r="B23">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" t="s">
-        <v>29</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1857,13 +1898,10 @@
       <c r="R23">
         <v>200</v>
       </c>
-      <c r="W23">
-        <v>0.26649352712254798</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -1914,24 +1952,32 @@
         <v>14.446006475136215</v>
       </c>
       <c r="W24">
-        <v>2.6132419668487818</v>
+        <v>1.1262520868113521</v>
       </c>
       <c r="Y24">
-        <v>0.52264839336975633</v>
+        <v>0.22525041736227042</v>
       </c>
       <c r="AA24">
-        <v>27.640009341645765</v>
+        <v>64.133095264825599</v>
       </c>
       <c r="AB24">
-        <v>28.234809680490908</v>
+        <v>56.617995720387242</v>
       </c>
       <c r="AC24">
-        <v>2.5696471674260941</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+        <v>7.5150995444383959</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" ref="AD24" si="12">AVERAGE(Y24:Y26)</f>
+        <v>0.25972454090150249</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" ref="AE24" si="13">_xlfn.STDEV.S(Y24:Y26)/SQRT(COUNT(Y24:Y26))</f>
+        <v>3.4474123539232161E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>10</v>
@@ -1979,18 +2025,18 @@
         <v>14.239078997547571</v>
       </c>
       <c r="W25">
-        <v>2.9956847856282987</v>
+        <v>1.4709933222036728</v>
       </c>
       <c r="Y25">
-        <v>0.59913695712565973</v>
+        <v>0.29419866444073456</v>
       </c>
       <c r="AA25">
-        <v>24.111359353361319</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
+        <v>49.102896175948892</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>10</v>
@@ -2037,19 +2083,10 @@
       <c r="S26">
         <v>18.63628789630625</v>
       </c>
-      <c r="W26">
-        <v>2.1919066580238908</v>
-      </c>
-      <c r="Y26">
-        <v>0.43838133160477816</v>
-      </c>
-      <c r="AA26">
-        <v>32.953060346465634</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -2100,24 +2137,32 @@
         <v>20.153756065289631</v>
       </c>
       <c r="W27">
-        <v>3.6050004630058337</v>
+        <v>2.0202420701168613</v>
       </c>
       <c r="Y27">
-        <v>0.72100009260116671</v>
+        <v>0.40404841402337227</v>
       </c>
       <c r="AA27">
-        <v>27.952501354861848</v>
+        <v>49.879557413938599</v>
       </c>
       <c r="AB27">
-        <v>28.243176499703893</v>
+        <v>50.85040032462458</v>
       </c>
       <c r="AC27">
-        <v>1.0094626574901577</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+        <v>2.9667269138324595</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" ref="AD27" si="14">AVERAGE(Y27:Y29)</f>
+        <v>0.39898441847523652</v>
+      </c>
+      <c r="AE27">
+        <f t="shared" ref="AE27" si="15">_xlfn.STDEV.S(Y27:Y29)/SQRT(COUNT(Y27:Y29))</f>
+        <v>2.2743822824477452E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <v>10</v>
@@ -2165,18 +2210,18 @@
         <v>20.5503670640012</v>
       </c>
       <c r="W28">
-        <v>3.3457171960366701</v>
+        <v>1.7865191986644409</v>
       </c>
       <c r="Y28">
-        <v>0.66914343920733399</v>
+        <v>0.35730383973288815</v>
       </c>
       <c r="AA28">
-        <v>30.118738202325844</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
+        <v>56.405092316825083</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>10</v>
@@ -2224,18 +2269,18 @@
         <v>23.136960533859241</v>
       </c>
       <c r="W29">
-        <v>3.7800166682100191</v>
+        <v>2.1780050083472453</v>
       </c>
       <c r="Y29">
-        <v>0.75600333364200378</v>
+        <v>0.43560100166944904</v>
       </c>
       <c r="AA29">
-        <v>26.658289941923982</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+        <v>46.266551243110051</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>10</v>
@@ -2285,25 +2330,24 @@
       <c r="U30">
         <v>19.739901110112346</v>
       </c>
-      <c r="W30">
-        <v>6.7629918247352041</v>
-      </c>
-      <c r="Y30">
-        <v>1.3525983649470408</v>
-      </c>
-      <c r="AA30">
-        <v>14.594059568366575</v>
-      </c>
       <c r="AB30">
-        <v>19.152282045714049</v>
+        <v>55.514181637411369</v>
       </c>
       <c r="AC30">
-        <v>2.2802919479261115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+        <v>2.185956290890676</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" ref="AD30" si="16">AVERAGE(Y30:Y32)</f>
+        <v>0.35613522537562597</v>
+      </c>
+      <c r="AE30">
+        <f t="shared" ref="AE30" si="17">_xlfn.STDEV.S(Y30:Y32)/SQRT(COUNT(Y30:Y32))</f>
+        <v>1.4023372287145175E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <v>10</v>
@@ -2351,18 +2395,18 @@
         <v>16.980868075597098</v>
       </c>
       <c r="W31">
-        <v>4.6328420120011229</v>
+        <v>1.710559265442404</v>
       </c>
       <c r="Y31">
-        <v>0.92656840240022453</v>
+        <v>0.3421118530884808</v>
       </c>
       <c r="AA31">
-        <v>21.304310679035911</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+        <v>57.700137928302041</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>10</v>
@@ -2410,18 +2454,18 @@
         <v>17.394723030774387</v>
       </c>
       <c r="W32">
-        <v>4.5782227860335825</v>
+        <v>1.8507929883138559</v>
       </c>
       <c r="Y32">
-        <v>0.91564455720671645</v>
+        <v>0.37015859766277115</v>
       </c>
       <c r="AA32">
-        <v>21.558475889739661</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
+        <v>53.328225346520689</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B33">
         <v>100</v>
@@ -2472,24 +2516,32 @@
         <v>76.001557582452619</v>
       </c>
       <c r="W33">
-        <v>3.6050004630058337</v>
+        <v>2.0202420701168613</v>
       </c>
       <c r="Y33">
-        <v>0.72100009260116671</v>
+        <v>0.40404841402337227</v>
       </c>
       <c r="AA33">
-        <v>105.41130072294479</v>
+        <v>188.10012598652668</v>
       </c>
       <c r="AB33">
-        <v>106.50746183985682</v>
+        <v>191.76125858835942</v>
       </c>
       <c r="AC33">
-        <v>3.8067710079466686</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
+        <v>11.187783837543899</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" ref="AD33" si="18">AVERAGE(Y33:Y35)</f>
+        <v>0.39898441847523652</v>
+      </c>
+      <c r="AE33">
+        <f t="shared" ref="AE33" si="19">_xlfn.STDEV.S(Y33:Y35)/SQRT(COUNT(Y33:Y35))</f>
+        <v>2.2743822824477452E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B34">
         <v>100</v>
@@ -2537,18 +2589,18 @@
         <v>53.929293306330663</v>
       </c>
       <c r="W34">
-        <v>3.3457171960366701</v>
+        <v>1.7865191986644409</v>
       </c>
       <c r="Y34">
-        <v>0.66914343920733399</v>
+        <v>0.35730383973288815</v>
       </c>
       <c r="AA34">
-        <v>113.58036727145367</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
+        <v>212.70848261599869</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B35">
         <v>100</v>
@@ -2596,18 +2648,18 @@
         <v>98.418700987888997</v>
       </c>
       <c r="W35">
-        <v>3.7800166682100191</v>
+        <v>2.1780050083472453</v>
       </c>
       <c r="Y35">
-        <v>0.75600333364200378</v>
+        <v>0.43560100166944904</v>
       </c>
       <c r="AA35">
-        <v>100.53071752517197</v>
-      </c>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
+        <v>174.47516716255294</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B36">
         <v>100</v>
@@ -2657,25 +2709,24 @@
       <c r="U36">
         <v>62.853434290744083</v>
       </c>
-      <c r="W36">
-        <v>6.7629918247352041</v>
-      </c>
-      <c r="Y36">
-        <v>1.3525983649470408</v>
-      </c>
-      <c r="AA36">
-        <v>46.468660557049418</v>
-      </c>
       <c r="AB36">
-        <v>60.982407883563837</v>
+        <v>176.76162348979511</v>
       </c>
       <c r="AC36">
-        <v>7.2606331365694583</v>
-      </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
+        <v>6.9602608100985464</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" ref="AD36" si="20">AVERAGE(Y36:Y38)</f>
+        <v>0.35613522537562597</v>
+      </c>
+      <c r="AE36">
+        <f t="shared" ref="AE36" si="21">_xlfn.STDEV.S(Y36:Y38)/SQRT(COUNT(Y36:Y38))</f>
+        <v>1.4023372287145175E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B37">
         <v>100</v>
@@ -2723,18 +2774,18 @@
         <v>162.04890034639686</v>
       </c>
       <c r="W37">
-        <v>4.6328420120011229</v>
+        <v>1.710559265442404</v>
       </c>
       <c r="Y37">
-        <v>0.92656840240022453</v>
+        <v>0.3421118530884808</v>
       </c>
       <c r="AA37">
-        <v>67.834640300625097</v>
-      </c>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
+        <v>183.72188429989365</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B38">
         <v>100</v>
@@ -2782,18 +2833,18 @@
         <v>0</v>
       </c>
       <c r="W38">
-        <v>4.5782227860335825</v>
+        <v>1.8507929883138559</v>
       </c>
       <c r="Y38">
-        <v>0.91564455720671645</v>
+        <v>0.37015859766277115</v>
       </c>
       <c r="AA38">
-        <v>68.643922793016998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
+        <v>169.80136267969655</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -2844,10 +2895,10 @@
         <v>0</v>
       </c>
       <c r="W39">
-        <v>0.152412040346279</v>
+        <v>0.38228155339805847</v>
       </c>
       <c r="Y39">
-        <v>3.0482408069255802E-2</v>
+        <v>7.64563106796117E-2</v>
       </c>
       <c r="AA39">
         <v>0</v>
@@ -2858,10 +2909,18 @@
       <c r="AC39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD39">
+        <f t="shared" ref="AD39" si="22">AVERAGE(Y39:Y41)</f>
+        <v>3.9690434505809391E-2</v>
+      </c>
+      <c r="AE39">
+        <f t="shared" ref="AE39" si="23">_xlfn.STDEV.S(Y39:Y41)/SQRT(COUNT(Y39:Y41))</f>
+        <v>2.1226788505937219E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B40">
         <v>10</v>
@@ -2909,18 +2968,18 @@
         <v>0</v>
       </c>
       <c r="W40">
-        <v>0.16825669128742701</v>
+        <v>1.4622791660035264E-2</v>
       </c>
       <c r="Y40">
-        <v>3.3651338257485404E-2</v>
+        <v>2.9245583320070528E-3</v>
       </c>
       <c r="AA40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B41">
         <v>10</v>
@@ -2968,18 +3027,18 @@
         <v>0</v>
       </c>
       <c r="W41">
-        <v>0.26649352712254798</v>
+        <v>0.19845217252904709</v>
       </c>
       <c r="Y41">
-        <v>5.3298705424509596E-2</v>
+        <v>3.9690434505809419E-2</v>
       </c>
       <c r="AA41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B42">
         <v>10</v>
@@ -3030,10 +3089,10 @@
         <v>0</v>
       </c>
       <c r="W42">
-        <v>1.8742846559866653</v>
+        <v>0.35721391055228413</v>
       </c>
       <c r="Y42">
-        <v>0.37485693119733304</v>
+        <v>7.1442782110456821E-2</v>
       </c>
       <c r="AA42">
         <v>0</v>
@@ -3044,10 +3103,18 @@
       <c r="AC42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AD42">
+        <f t="shared" ref="AD42" si="24">AVERAGE(Y42:Y44)</f>
+        <v>8.759748527773363E-2</v>
+      </c>
+      <c r="AE42">
+        <f t="shared" ref="AE42" si="25">_xlfn.STDEV.S(Y42:Y44)/SQRT(COUNT(Y42:Y44))</f>
+        <v>1.3724462034582942E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B43">
         <v>10</v>
@@ -3095,18 +3162,18 @@
         <v>0</v>
       </c>
       <c r="W43">
-        <v>2.2891378831373275</v>
+        <v>0.57446681521566179</v>
       </c>
       <c r="Y43">
-        <v>0.45782757662746548</v>
+        <v>0.11489336304313236</v>
       </c>
       <c r="AA43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B44">
         <v>10</v>
@@ -3154,16 +3221,16 @@
         <v>0</v>
       </c>
       <c r="W44">
-        <v>1.932623391054727</v>
+        <v>0.38228155339805847</v>
       </c>
       <c r="Y44">
-        <v>0.38652467821094538</v>
+        <v>7.64563106796117E-2</v>
       </c>
       <c r="AA44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -3216,22 +3283,30 @@
         <v>32.052086026636623</v>
       </c>
       <c r="W45">
-        <v>3.1512547458097968</v>
+        <v>1.6112270450751254</v>
       </c>
       <c r="Y45">
-        <v>0.63025094916195934</v>
+        <v>0.32224540901502507</v>
       </c>
       <c r="AA45">
-        <v>50.856069426402414</v>
+        <v>99.464833725969868</v>
       </c>
       <c r="AB45">
-        <v>45.105342717129055</v>
+        <v>88.942463896489159</v>
       </c>
       <c r="AC45">
-        <v>3.0790747898530002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
+        <v>10.522369829480638</v>
+      </c>
+      <c r="AD45">
+        <f t="shared" ref="AD45" si="26">AVERAGE(Y45:Y47)</f>
+        <v>0.36548414023372289</v>
+      </c>
+      <c r="AE45">
+        <f t="shared" ref="AE45" si="27">_xlfn.STDEV.S(Y45:Y47)/SQRT(COUNT(Y45:Y47))</f>
+        <v>4.3238731218697521E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -3281,16 +3356,16 @@
         <v>35.50087731978067</v>
       </c>
       <c r="W46">
-        <v>3.6309287897027498</v>
+        <v>2.0436143572621033</v>
       </c>
       <c r="Y46">
-        <v>0.72618575794054996</v>
+        <v>0.40872287145242064</v>
       </c>
       <c r="AA46">
-        <v>44.137585564244297</v>
-      </c>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+        <v>78.420094067008435</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -3339,17 +3414,8 @@
       <c r="S47">
         <v>31.15540029041917</v>
       </c>
-      <c r="W47">
-        <v>3.9744791184368924</v>
-      </c>
-      <c r="Y47">
-        <v>0.79489582368737843</v>
-      </c>
-      <c r="AA47">
-        <v>40.322373160740455</v>
-      </c>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -3402,22 +3468,30 @@
         <v>35.155998190466278</v>
       </c>
       <c r="W48">
-        <v>6.1731041842857657</v>
+        <v>2.9376043405676127</v>
       </c>
       <c r="Y48">
-        <v>1.2346208368571532</v>
+        <v>0.58752086811352255</v>
       </c>
       <c r="AA48">
-        <v>28.475137581477462</v>
+        <v>59.837871467185622</v>
       </c>
       <c r="AB48">
-        <v>32.157732233914317</v>
+        <v>60.017474883295243</v>
       </c>
       <c r="AC48">
-        <v>3.932758153521509</v>
-      </c>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
+        <v>0.17960341610962158</v>
+      </c>
+      <c r="AD48">
+        <f t="shared" ref="AD48" si="28">AVERAGE(Y48:Y50)</f>
+        <v>0.58576794657762932</v>
+      </c>
+      <c r="AE48">
+        <f t="shared" ref="AE48" si="29">_xlfn.STDEV.S(Y48:Y50)/SQRT(COUNT(Y48:Y50))</f>
+        <v>1.7529215358932369E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -3466,17 +3540,8 @@
       <c r="S49">
         <v>37.311492748681317</v>
       </c>
-      <c r="W49">
-        <v>4.392517417743945</v>
-      </c>
-      <c r="Y49">
-        <v>0.87850348354878904</v>
-      </c>
-      <c r="AA49">
-        <v>40.018052117961616</v>
-      </c>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -3526,18 +3591,18 @@
         <v>37.104565271092675</v>
       </c>
       <c r="W50">
-        <v>6.2823426362208474</v>
+        <v>2.9200751252086805</v>
       </c>
       <c r="Y50">
-        <v>1.2564685272441696</v>
+        <v>0.58401502504173608</v>
       </c>
       <c r="AA50">
-        <v>27.980007002303857</v>
-      </c>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
+        <v>60.197078299404865</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B51">
         <v>100</v>
@@ -3588,24 +3653,32 @@
         <v>117.90437179415291</v>
       </c>
       <c r="W51">
-        <v>3.1512547458097968</v>
+        <v>1.6112270450751254</v>
       </c>
       <c r="Y51">
-        <v>0.63025094916195934</v>
+        <v>0.32224540901502507</v>
       </c>
       <c r="AA51">
-        <v>187.0752784282667</v>
+        <v>365.88379072502312</v>
       </c>
       <c r="AB51">
-        <v>165.9210914760273</v>
+        <v>327.17699942602144</v>
       </c>
       <c r="AC51">
-        <v>11.326450905664391</v>
-      </c>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
+        <v>38.706791299001615</v>
+      </c>
+      <c r="AD51">
+        <f t="shared" ref="AD51" si="30">AVERAGE(Y51:Y53)</f>
+        <v>0.36548414023372289</v>
+      </c>
+      <c r="AE51">
+        <f t="shared" ref="AE51" si="31">_xlfn.STDEV.S(Y51:Y53)/SQRT(COUNT(Y51:Y53))</f>
+        <v>4.3238731218697521E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B52">
         <v>100</v>
@@ -3653,18 +3726,18 @@
         <v>144.97738344533377</v>
       </c>
       <c r="W52">
-        <v>3.6309287897027498</v>
+        <v>2.0436143572621033</v>
       </c>
       <c r="Y52">
-        <v>0.72618575794054996</v>
+        <v>0.40872287145242064</v>
       </c>
       <c r="AA52">
-        <v>162.36117343932443</v>
-      </c>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
+        <v>288.4702081270197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B53">
         <v>100</v>
@@ -3711,19 +3784,10 @@
       <c r="S53">
         <v>139.28687781164606</v>
       </c>
-      <c r="W53">
-        <v>3.9744791184368924</v>
-      </c>
-      <c r="Y53">
-        <v>0.79489582368737843</v>
-      </c>
-      <c r="AA53">
-        <v>148.32682256049074</v>
-      </c>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B54">
         <v>100</v>
@@ -3774,24 +3838,32 @@
         <v>225.33422057559028</v>
       </c>
       <c r="W54">
-        <v>6.1731041842857657</v>
+        <v>2.9376043405676127</v>
       </c>
       <c r="Y54">
-        <v>1.2346208368571532</v>
+        <v>0.58752086811352255</v>
       </c>
       <c r="AA54">
-        <v>182.51289290499935</v>
+        <v>383.53398628906319</v>
       </c>
       <c r="AB54">
-        <v>206.11667713570077</v>
+        <v>384.68516383670431</v>
       </c>
       <c r="AC54">
-        <v>25.207220356393975</v>
-      </c>
-    </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.35">
+        <v>1.1511775476410833</v>
+      </c>
+      <c r="AD54">
+        <f t="shared" ref="AD54" si="32">AVERAGE(Y54:Y56)</f>
+        <v>0.58576794657762932</v>
+      </c>
+      <c r="AE54">
+        <f t="shared" ref="AE54" si="33">_xlfn.STDEV.S(Y54:Y56)/SQRT(COUNT(Y54:Y56))</f>
+        <v>1.7529215358932369E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B55">
         <v>100</v>
@@ -3838,19 +3910,10 @@
       <c r="S55">
         <v>229.30033056270597</v>
       </c>
-      <c r="W55">
-        <v>4.392517417743945</v>
-      </c>
-      <c r="Y55">
-        <v>0.87850348354878904</v>
-      </c>
-      <c r="AA55">
-        <v>256.49781110182244</v>
-      </c>
-    </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B56">
         <v>100</v>
@@ -3898,13 +3961,13 @@
         <v>183.25896679923281</v>
       </c>
       <c r="W56">
-        <v>6.2823426362208474</v>
+        <v>2.9200751252086805</v>
       </c>
       <c r="Y56">
-        <v>1.2564685272441696</v>
+        <v>0.58401502504173608</v>
       </c>
       <c r="AA56">
-        <v>179.33932740028041</v>
+        <v>385.83634138434536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>